<commit_message>
solved the formcode.php and thus the comment section
</commit_message>
<xml_diff>
--- a/davidmszabo/Time Sheet.xlsx
+++ b/davidmszabo/Time Sheet.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Start time</t>
   </si>
@@ -58,13 +58,16 @@
   </si>
   <si>
     <t>Modifying the template</t>
+  </si>
+  <si>
+    <t>Solved the php include stuff</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -94,6 +97,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -117,11 +126,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -130,6 +142,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -455,39 +472,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F9" sqref="F9:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="16">
+    <row r="2" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2">
@@ -499,7 +517,7 @@
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="16">
+    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2">
@@ -513,7 +531,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>0.75</v>
       </c>
@@ -534,7 +552,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="26" customHeight="1">
+    <row r="5" spans="1:6" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>0.70833333333333337</v>
       </c>
@@ -555,9 +573,30 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.57916666666666672</v>
+      </c>
+      <c r="C6" s="2">
+        <f>B6-A6</f>
+        <v>3.7500000000000089E-2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>41787</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>